<commit_message>
modication du html page 2 pour remettre barre de recherche
</commit_message>
<xml_diff>
--- a/P4_rosamond_fabrice/P4_01_analyse.xlsx
+++ b/P4_rosamond_fabrice/P4_01_analyse.xlsx
@@ -11,6 +11,7 @@
     <sheet name="ELEMENTS RETENUS CRITERES" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="125725" concurrentCalc="0"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="138">
   <si>
     <t>Catégorie</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Mise en œuvre moins urgente</t>
   </si>
   <si>
-    <t xml:space="preserve">1.3.5 Identify Input purpose </t>
-  </si>
-  <si>
     <t>Dans les formulaires, indiquer une valeur d'autocompletion (Ex: Nom - Prénom)</t>
   </si>
   <si>
@@ -95,9 +93,6 @@
     <t>Espacer suffisament le texte et tester le texte du site avec l'extension "zoom text only" en augmentant la taille du texte jusqu'à 200% afin de voir s'il reste des chevauchements. On peut aussi réorganiser les parties concernées.</t>
   </si>
   <si>
-    <t>1.1.1 non-text content guide WCAG</t>
-  </si>
-  <si>
     <t>Afin que les malvoyants ou non voyants aient accès à l'image, il faut un texte alternatif cohérent et qui décrit l'image présente, or ce n'est pas le cas.</t>
   </si>
   <si>
@@ -119,27 +114,6 @@
     <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Utilisation de Pingdom pour analyser la cinétique de chargement de la page et des images en particulier ainsi que lien vers le cours sur allégez les pages de votre site : </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
-    </r>
-  </si>
-  <si>
     <t>Afin d'enrichir au maximum l'expérience des malvoyants, il faut un texte alternatif qui décrit l'icône présente à l'écran, sans quoi il passera à côté de certains éléments qui  font la cohérence du site.</t>
   </si>
   <si>
@@ -158,15 +132,9 @@
     <t>Les utilisateurs ayant une vision faible ou des difficultés à distinguer les nuances de couleur auront du mal à lire le texte inscrit sur le bouton.</t>
   </si>
   <si>
-    <t>1.4.3 Contrast (Minimum) du guide WCAG</t>
-  </si>
-  <si>
     <t>D'une manière générale, il est conseillé de compresser les images. On peut utiliser des outils de compression comme imageOptim, PNG gauntlet ou https://compressor.io/</t>
   </si>
   <si>
-    <t>1.1.1 non-text content guide wcag et utilisation du Contrast Colour Analyzer pour connaître le degré de contraste entre les 2 couleurs.</t>
-  </si>
-  <si>
     <t>Il faut trouver une couleur de fond présentant suffisamment de contraste avec la couleur du texte, tout en restant dans la charte graphique de La Chouette Agence. Actuellement ce contraste est à 2,2 : 1 et il devrait être au minimum à 3:1 pour les textes de cette taille.</t>
   </si>
   <si>
@@ -182,32 +150,6 @@
     <t>2.4.7 Focus visible</t>
   </si>
   <si>
-    <r>
-      <t>1.4.4. Resize text image du content guide WCAG et "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>extension chrome zoom text image"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
     <t>Dans le cas ou les scripts peuvent être exécutés dès qu'ils sont disponibles, mieux vaut privilégier une exécution asynchrone du javascript.</t>
   </si>
   <si>
@@ -271,9 +213,6 @@
     <t>Il faut réaliser les adaptations nécessaires afin que tous les éléments soient présents à l'écran quand on consulte le site depuis un téléphone portable.</t>
   </si>
   <si>
-    <t>Lien vers le cours sur la création d'iun contenu web accessible : https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941560-annotez-vos-maquettes-a-laide-dinformations-daccessibilite</t>
-  </si>
-  <si>
     <t>Absence de balise structurante html.</t>
   </si>
   <si>
@@ -433,9 +372,6 @@
     <t>Les utilisateurs de technologie d'assistance n'auront pas assez d'information sur les liens. Ils devront cliquer dessus pour savoir où ces liens les emmenent.</t>
   </si>
   <si>
-    <t>2.4.4 Link purpose (in context) du guide WCAG et http://www.handi-pratique.com/accessibilite-liens-title et également https://www.handi-pratique.com/nouvelle-version-referentiel-accessiweb</t>
-  </si>
-  <si>
     <t>Correctement nommer les class et les id utilisés, les simplifier et les rendre compréhensible, dans un but de maintenabilité du code.</t>
   </si>
   <si>
@@ -476,13 +412,34 @@
   </si>
   <si>
     <t>*Ce sont les éléments retenus</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-scale.html</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/text-equiv-all.html</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/visual-audio-contrast-contrast.html</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/6691346-concevez-un-contenu-web-accessible/6941560-annotez-vos-maquettes-a-laide-dinformations-daccessibilite</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/WCAG21/Understanding/identify-input-purpose.html</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/TR/UNDERSTANDING-WCAG20/navigation-mechanisms-refs.html</t>
+  </si>
+  <si>
+    <t>Utilisation de Pingdom pour analyser la cinétique de chargement de la page et des images en particulier ainsi que lien vers le cours sur allégez les pages de votre site : https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-si</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -522,14 +479,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
@@ -543,19 +492,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -733,7 +669,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -762,23 +698,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -807,6 +734,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1017,9 +956,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -1034,22 +973,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="38.4" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1"/>
@@ -1078,19 +1017,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="E2" s="7">
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:26" s="8" customFormat="1" ht="46.8">
@@ -1098,19 +1037,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="E3" s="7">
         <v>2</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="8" customFormat="1" ht="78">
@@ -1118,79 +1057,80 @@
         <v>7</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="8" customFormat="1" ht="62.4">
-      <c r="A5" s="14" t="s">
+      <c r="F4" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="28"/>
+    </row>
+    <row r="5" spans="1:26" s="8" customFormat="1" ht="46.8">
+      <c r="A5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E5" s="7">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" s="8" customFormat="1" ht="106.8">
+      <c r="F5" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="8" customFormat="1" ht="75">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" s="8" customFormat="1" ht="109.2">
+      <c r="F6" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" s="8" customFormat="1" ht="93.6">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>40</v>
+      <c r="F7" s="14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="8" customFormat="1" ht="78">
@@ -1198,19 +1138,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>42</v>
+      <c r="F8" s="14" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="8" customFormat="1" ht="78">
@@ -1218,19 +1158,19 @@
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E9" s="7">
         <v>3</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>53</v>
+      <c r="F9" s="14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="8" customFormat="1" ht="93.6">
@@ -1238,79 +1178,79 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" s="8" customFormat="1" ht="93.6">
+      <c r="F10" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="8" customFormat="1" ht="90">
       <c r="A11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E11" s="7">
         <v>2</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" s="8" customFormat="1" ht="78">
+      <c r="F11" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="8" customFormat="1" ht="75">
       <c r="A12" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E12" s="7">
         <v>3</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" s="8" customFormat="1" ht="78">
+      <c r="F12" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" s="8" customFormat="1" ht="46.8">
       <c r="A13" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E13" s="7">
         <v>2</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>70</v>
+      <c r="F13" s="14" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:26" s="8" customFormat="1" ht="78">
@@ -1318,19 +1258,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E14" s="7">
         <v>1</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>75</v>
+      <c r="F14" s="14" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="8" customFormat="1" ht="124.8">
@@ -1338,22 +1278,22 @@
         <v>6</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" s="8" customFormat="1" ht="78">
+      <c r="F15" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" s="8" customFormat="1" ht="75">
       <c r="A16" s="9" t="s">
         <v>6</v>
       </c>
@@ -1361,16 +1301,16 @@
         <v>9</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E16" s="7">
         <v>2</v>
       </c>
-      <c r="F16" s="7" t="s">
-        <v>60</v>
+      <c r="F16" s="14" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="8" customFormat="1" ht="31.2">
@@ -1381,16 +1321,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>37</v>
+      <c r="F17" s="30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="8" customFormat="1" ht="78">
@@ -1398,59 +1338,59 @@
         <v>6</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E18" s="7">
         <v>1</v>
       </c>
-      <c r="F18" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="11" customFormat="1" ht="62.4">
+      <c r="F18" s="31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="11" customFormat="1" ht="60">
       <c r="A19" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E19" s="7">
         <v>2</v>
       </c>
-      <c r="F19" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="11" customFormat="1" ht="46.8">
+      <c r="F19" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="11" customFormat="1" ht="45">
       <c r="A20" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="E20" s="7">
         <v>2</v>
       </c>
-      <c r="F20" s="7" t="s">
-        <v>79</v>
+      <c r="F20" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1" ht="62.4">
@@ -1458,19 +1398,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E21" s="7">
         <v>2</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>130</v>
+      <c r="F21" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" ht="62.4">
@@ -1478,59 +1418,59 @@
         <v>7</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E22" s="7">
         <v>2</v>
       </c>
-      <c r="F22" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" ht="78">
+      <c r="F22" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" ht="75">
       <c r="A23" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" ht="46.8">
+      <c r="F23" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" ht="45">
       <c r="A24" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E24" s="7">
         <v>2</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>57</v>
+      <c r="F24" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1" ht="62.4">
@@ -1538,39 +1478,39 @@
         <v>6</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E25" s="7">
         <v>2</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" ht="62.4">
+      <c r="F25" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" ht="46.8">
       <c r="A26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E26" s="7">
         <v>2</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>47</v>
+      <c r="F26" s="14" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="11" customFormat="1" ht="62.4">
@@ -1578,19 +1518,19 @@
         <v>7</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E27" s="7">
         <v>2</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>124</v>
+      <c r="F27" s="14" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1" ht="46.8">
@@ -1598,19 +1538,19 @@
         <v>6</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="E28" s="7">
         <v>2</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>112</v>
+      <c r="F28" s="14" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="11" customFormat="1" ht="62.4">
@@ -1618,39 +1558,39 @@
         <v>7</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E29" s="7">
         <v>2</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" ht="109.2">
+      <c r="F29" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" ht="93.6">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E30" s="7">
         <v>1</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>82</v>
+      <c r="F30" s="14" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1" ht="46.8">
@@ -1658,115 +1598,115 @@
         <v>7</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="E31" s="7">
         <v>2</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="8" customFormat="1" ht="78">
+      <c r="F31" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" ht="75">
       <c r="A32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="E32" s="7">
         <v>2</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="8" customFormat="1" ht="46.8">
+      <c r="F32" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" ht="45">
       <c r="A33" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E33" s="7">
         <v>2</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" ht="78.599999999999994" thickBot="1">
+      <c r="A34" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="19" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" s="8" customFormat="1" ht="78.599999999999994" thickBot="1">
-      <c r="A34" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>119</v>
+      <c r="C34" s="19" t="s">
+        <v>112</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E34" s="7">
         <v>3</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>79</v>
+      <c r="F34" s="14" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A35" s="23">
+      <c r="A35" s="20">
         <v>1</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="25" t="s">
-        <v>138</v>
+      <c r="C35" s="22" t="s">
+        <v>130</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A36" s="26">
+      <c r="A36" s="23">
         <v>2</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="27"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A37" s="28">
+      <c r="A37" s="25">
         <v>3</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="30"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -3097,9 +3037,40 @@
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F7" r:id="rId5"/>
+    <hyperlink ref="F8" r:id="rId6"/>
+    <hyperlink ref="F13" r:id="rId7"/>
+    <hyperlink ref="F17" r:id="rId8"/>
+    <hyperlink ref="F21" r:id="rId9"/>
+    <hyperlink ref="F22" r:id="rId10"/>
+    <hyperlink ref="F26" r:id="rId11"/>
+    <hyperlink ref="F27" r:id="rId12"/>
+    <hyperlink ref="F29" r:id="rId13"/>
+    <hyperlink ref="F31" r:id="rId14"/>
+    <hyperlink ref="F6" r:id="rId15"/>
+    <hyperlink ref="F9" r:id="rId16"/>
+    <hyperlink ref="F10" r:id="rId17"/>
+    <hyperlink ref="F11" r:id="rId18"/>
+    <hyperlink ref="F12" r:id="rId19"/>
+    <hyperlink ref="F14" r:id="rId20"/>
+    <hyperlink ref="F15" r:id="rId21"/>
+    <hyperlink ref="F16" r:id="rId22"/>
+    <hyperlink ref="F18" r:id="rId23"/>
+    <hyperlink ref="F19" r:id="rId24"/>
+    <hyperlink ref="F20" r:id="rId25"/>
+    <hyperlink ref="F23" r:id="rId26"/>
+    <hyperlink ref="F24" r:id="rId27"/>
+    <hyperlink ref="F25" r:id="rId28"/>
+    <hyperlink ref="F28" r:id="rId29"/>
+    <hyperlink ref="F30" r:id="rId30"/>
+    <hyperlink ref="F32" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
+    <hyperlink ref="F34" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="53" orientation="landscape" verticalDpi="300" r:id="rId34"/>
 </worksheet>
 </file>
 

</xml_diff>